<commit_message>
- Updating shiva temples with contact numbers.
</commit_message>
<xml_diff>
--- a/nama_shi-vaya.xlsx
+++ b/nama_shi-vaya.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Mohindar\shiva_temples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F47D66-D8A5-41A4-B4D9-6B81779C85DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E08E781-6CC4-4EC8-ACAB-5491B8F91A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13935" yWindow="0" windowWidth="13935" windowHeight="16200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="281">
   <si>
     <t>Temple</t>
   </si>
@@ -853,12 +853,48 @@
   <si>
     <t>+01-9445356399</t>
   </si>
+  <si>
+    <t>Shri Aavundeeswarar Swamy</t>
+  </si>
+  <si>
+    <t>Shri Amrithambika Ambal</t>
+  </si>
+  <si>
+    <t>Nemam</t>
+  </si>
+  <si>
+    <t>Shri Aavundeeswarar Swamy Temple, Nemam</t>
+  </si>
+  <si>
+    <t>அருள்மிகு ஸ்ரீ அமிர்தாம்பிகை அம்பாள் உடனுறை ஸ்ரீ ஆவுண்டீஸ்வரர்  ஸ்வாமி திருக்கோவில்</t>
+  </si>
+  <si>
+    <t>+91-9840770248</t>
+  </si>
+  <si>
+    <t>+91-9555770579</t>
+  </si>
+  <si>
+    <t>+91-9444943644</t>
+  </si>
+  <si>
+    <t>+91-9444325093</t>
+  </si>
+  <si>
+    <t>+91-9894486890</t>
+  </si>
+  <si>
+    <t>+91-9444164108</t>
+  </si>
+  <si>
+    <t>+91-9443253325</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -922,6 +958,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -950,7 +993,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -976,6 +1019,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1359,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N53"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A39"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1582,7 +1626,9 @@
         <v>134</v>
       </c>
       <c r="I7" s="10"/>
-      <c r="J7" s="11"/>
+      <c r="J7" s="11" t="s">
+        <v>280</v>
+      </c>
       <c r="K7" s="10"/>
       <c r="L7" s="11"/>
     </row>
@@ -2584,7 +2630,9 @@
         <v>94</v>
       </c>
       <c r="I37" s="10"/>
-      <c r="J37" s="11"/>
+      <c r="J37" s="11" t="s">
+        <v>279</v>
+      </c>
       <c r="K37" s="10"/>
       <c r="L37" s="11"/>
     </row>
@@ -2614,7 +2662,9 @@
         <v>125</v>
       </c>
       <c r="I38" s="10"/>
-      <c r="J38" s="11"/>
+      <c r="J38" s="11" t="s">
+        <v>278</v>
+      </c>
       <c r="K38" s="10"/>
       <c r="L38" s="11"/>
     </row>
@@ -2666,7 +2716,7 @@
       <c r="B44" s="2"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="50" spans="2:8">
+    <row r="50" spans="2:14">
       <c r="B50" s="12" t="s">
         <v>165</v>
       </c>
@@ -2687,7 +2737,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="51" spans="2:8">
+    <row r="51" spans="2:14">
       <c r="B51" s="13" t="s">
         <v>250</v>
       </c>
@@ -2708,7 +2758,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="52" spans="2:8">
+    <row r="52" spans="2:14">
       <c r="B52" s="15" t="s">
         <v>253</v>
       </c>
@@ -2729,7 +2779,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="53" spans="2:8">
+    <row r="53" spans="2:14">
       <c r="B53" s="16" t="s">
         <v>259</v>
       </c>
@@ -2748,6 +2798,41 @@
       <c r="G53" s="10"/>
       <c r="H53" s="7" t="s">
         <v>263</v>
+      </c>
+      <c r="J53" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="L53" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="N53" s="9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14">
+      <c r="B54" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="C54" t="s">
+        <v>270</v>
+      </c>
+      <c r="D54" t="s">
+        <v>269</v>
+      </c>
+      <c r="E54" t="s">
+        <v>271</v>
+      </c>
+      <c r="F54" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="I54" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="J54" s="9" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -2833,8 +2918,9 @@
     <hyperlink ref="H53" r:id="rId76" xr:uid="{B05C7F4C-E96E-4BB7-8B7B-AB884E049D0F}"/>
     <hyperlink ref="G36" r:id="rId77" xr:uid="{52952E4F-E22A-4E75-9D81-5C55ABC8802D}"/>
     <hyperlink ref="H36" r:id="rId78" xr:uid="{25FB256E-8D4E-41F3-BFDA-6C0AE68F6641}"/>
+    <hyperlink ref="H54" r:id="rId79" xr:uid="{4966F435-DF39-4F95-A013-A60EB2686F6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId79"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId80"/>
 </worksheet>
 </file>
</xml_diff>